<commit_message>
Add new user stories
</commit_message>
<xml_diff>
--- a/DPB.xlsx
+++ b/DPB.xlsx
@@ -209,6 +209,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -231,6 +232,7 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -239,6 +241,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -246,12 +249,14 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -259,6 +264,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -328,11 +334,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -365,7 +371,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -373,8 +379,16 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -395,12 +409,18 @@
     <dxf>
       <font>
         <name val="Calibri"/>
+        <charset val="1"/>
         <family val="2"/>
         <b val="0"/>
         <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
         <color rgb="FF000000"/>
         <sz val="11"/>
+        <u val="none"/>
       </font>
+      <numFmt numFmtId="164" formatCode="General"/>
       <fill>
         <patternFill>
           <bgColor rgb="FFCCCCCC"/>
@@ -408,10 +428,10 @@
       </fill>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <border diagonalUp="false" diagonalDown="false">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
+        <left style="thin"/>
+        <right style="thin"/>
+        <top style="thin"/>
+        <bottom style="thin"/>
         <diagonal/>
       </border>
     </dxf>
@@ -487,11 +507,11 @@
   </sheetPr>
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.92"/>
@@ -552,11 +572,11 @@
   </sheetPr>
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.89"/>
@@ -678,14 +698,14 @@
       <c r="D7" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="10" t="s">
         <v>24</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" s="10" customFormat="true" ht="60.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" s="11" customFormat="true" ht="60.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
         <v>27</v>
       </c>
@@ -786,72 +806,72 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="56.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="9" t="s">
+      <c r="B13" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="F13" s="12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="61.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="9" t="s">
+      <c r="B14" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="F14" s="12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="42" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="9" t="s">
+      <c r="B15" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="F15" s="9" t="s">
+      <c r="F15" s="12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="42" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
     </row>
     <row r="17" customFormat="false" ht="42" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="9"/>
@@ -926,17 +946,17 @@
   </sheetPr>
   <dimension ref="B2:B12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L28" activeCellId="0" sqref="L28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="8.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="13" t="s">
         <v>49</v>
       </c>
     </row>
@@ -961,7 +981,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="13" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>